<commit_message>
re-ordered bill data to be chronological
</commit_message>
<xml_diff>
--- a/SummitBillsExcel.xlsx
+++ b/SummitBillsExcel.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzastrow\Documents\GitHub\weather\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834AD941-B8A1-4B0A-88ED-A327F3E34E6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EEB312-9FB7-4944-ACB1-6F4B71374EC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{0FD02906-023E-41B2-84A8-9117E1316348}"/>
+    <workbookView xWindow="-28920" yWindow="4455" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD02906-023E-41B2-84A8-9117E1316348}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Vert" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="GasBills2" sheetId="5" r:id="rId1"/>
+    <sheet name="GasBills" sheetId="1" r:id="rId2"/>
+    <sheet name="Vert" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Stations" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="75">
   <si>
     <t>DateBill</t>
   </si>
@@ -255,6 +258,9 @@
   <si>
     <t>Cumberland, ME, US</t>
   </si>
+  <si>
+    <t>Gas</t>
+  </si>
 </sst>
 </file>
 
@@ -1653,7 +1659,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$F$1</c15:sqref>
@@ -1682,7 +1688,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$C$2:$D$24</c15:sqref>
@@ -1838,7 +1844,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$F$2:$F$24</c15:sqref>
@@ -1921,7 +1927,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-12A2-4A2B-A84C-DCCEB441A6E9}"/>
                   </c:ext>
@@ -1934,7 +1940,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$G$1</c15:sqref>
@@ -1963,7 +1969,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$C$2:$D$24</c15:sqref>
@@ -2119,7 +2125,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$G$2:$G$24</c15:sqref>
@@ -2202,7 +2208,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-12A2-4A2B-A84C-DCCEB441A6E9}"/>
                   </c:ext>
@@ -2215,7 +2221,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$J$1</c15:sqref>
@@ -2244,7 +2250,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$C$2:$D$24</c15:sqref>
@@ -2400,7 +2406,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$J$2:$J$24</c15:sqref>
@@ -2483,7 +2489,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-12A2-4A2B-A84C-DCCEB441A6E9}"/>
                   </c:ext>
@@ -2496,7 +2502,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$M$1</c15:sqref>
@@ -2527,7 +2533,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:multiLvlStrRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$C$2:$D$24</c15:sqref>
@@ -2683,7 +2689,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Vert!$M$2:$M$24</c15:sqref>
@@ -2766,7 +2772,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-12A2-4A2B-A84C-DCCEB441A6E9}"/>
                   </c:ext>
@@ -3497,6 +3503,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="663835368"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -5056,22 +5063,2057 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34037E50-BB0D-48F3-B9E8-18F906E40F64}">
+  <dimension ref="A1:X30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="23.61328125" customWidth="1"/>
+    <col min="2" max="24" width="14.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1">
+        <v>42711</v>
+      </c>
+      <c r="C1" s="1">
+        <v>42740</v>
+      </c>
+      <c r="D1" s="1">
+        <v>42772</v>
+      </c>
+      <c r="E1" s="1">
+        <v>42800</v>
+      </c>
+      <c r="F1" s="1">
+        <v>42831</v>
+      </c>
+      <c r="G1" s="1">
+        <v>42859</v>
+      </c>
+      <c r="H1" s="1">
+        <v>42892</v>
+      </c>
+      <c r="I1" s="1">
+        <v>42926</v>
+      </c>
+      <c r="J1" s="1">
+        <v>42954</v>
+      </c>
+      <c r="K1" s="1">
+        <v>42985</v>
+      </c>
+      <c r="L1" s="1">
+        <v>43013</v>
+      </c>
+      <c r="M1" s="1">
+        <v>43045</v>
+      </c>
+      <c r="N1" s="1">
+        <v>43075</v>
+      </c>
+      <c r="O1" s="1">
+        <v>43137</v>
+      </c>
+      <c r="P1" s="1">
+        <v>43165</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>43195</v>
+      </c>
+      <c r="R1" s="1">
+        <v>43229</v>
+      </c>
+      <c r="S1" s="1">
+        <v>43290</v>
+      </c>
+      <c r="T1" s="1">
+        <v>43353</v>
+      </c>
+      <c r="U1" s="1">
+        <v>43377</v>
+      </c>
+      <c r="V1" s="1">
+        <v>43411</v>
+      </c>
+      <c r="W1" s="1">
+        <v>43440</v>
+      </c>
+      <c r="X1" s="1">
+        <v>43472</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42709</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42739</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42769</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42797</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42830</v>
+      </c>
+      <c r="G3" s="1">
+        <v>42858</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42891</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42922</v>
+      </c>
+      <c r="J3" s="1">
+        <v>42950</v>
+      </c>
+      <c r="K3" s="1">
+        <v>42984</v>
+      </c>
+      <c r="L3" s="1">
+        <v>43012</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43042</v>
+      </c>
+      <c r="N3" s="1">
+        <v>43074</v>
+      </c>
+      <c r="O3" s="1">
+        <v>43136</v>
+      </c>
+      <c r="P3" s="1">
+        <v>43164</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>43194</v>
+      </c>
+      <c r="R3" s="1">
+        <v>43223</v>
+      </c>
+      <c r="S3" s="1">
+        <v>43286</v>
+      </c>
+      <c r="T3" s="1">
+        <v>43349</v>
+      </c>
+      <c r="U3" s="1">
+        <v>43376</v>
+      </c>
+      <c r="V3" s="1">
+        <v>43409</v>
+      </c>
+      <c r="W3" s="1">
+        <v>43439</v>
+      </c>
+      <c r="X3" s="1">
+        <v>43469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42677</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42709</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42739</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42769</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42797</v>
+      </c>
+      <c r="G4" s="1">
+        <v>42830</v>
+      </c>
+      <c r="H4" s="1">
+        <v>42858</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42891</v>
+      </c>
+      <c r="J4" s="1">
+        <v>42922</v>
+      </c>
+      <c r="K4" s="1">
+        <v>42950</v>
+      </c>
+      <c r="L4" s="1">
+        <v>42984</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43012</v>
+      </c>
+      <c r="N4" s="1">
+        <v>43042</v>
+      </c>
+      <c r="O4" s="1">
+        <v>43103</v>
+      </c>
+      <c r="P4" s="1">
+        <v>43136</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>43164</v>
+      </c>
+      <c r="R4" s="1">
+        <v>43194</v>
+      </c>
+      <c r="S4" s="1">
+        <v>43256</v>
+      </c>
+      <c r="T4" s="1">
+        <v>43315</v>
+      </c>
+      <c r="U4" s="1">
+        <v>43349</v>
+      </c>
+      <c r="V4" s="1">
+        <v>43376</v>
+      </c>
+      <c r="W4" s="1">
+        <v>43409</v>
+      </c>
+      <c r="X4" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>31</v>
+      </c>
+      <c r="J5">
+        <v>28</v>
+      </c>
+      <c r="K5">
+        <v>34</v>
+      </c>
+      <c r="L5">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>33</v>
+      </c>
+      <c r="P5">
+        <v>28</v>
+      </c>
+      <c r="Q5">
+        <v>30</v>
+      </c>
+      <c r="R5">
+        <v>29</v>
+      </c>
+      <c r="S5">
+        <v>30</v>
+      </c>
+      <c r="T5">
+        <v>34</v>
+      </c>
+      <c r="U5">
+        <v>27</v>
+      </c>
+      <c r="V5">
+        <v>33</v>
+      </c>
+      <c r="W5">
+        <v>30</v>
+      </c>
+      <c r="X5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2850</v>
+      </c>
+      <c r="C6">
+        <v>3073</v>
+      </c>
+      <c r="D6">
+        <v>3292</v>
+      </c>
+      <c r="E6">
+        <v>3488</v>
+      </c>
+      <c r="F6">
+        <v>3734</v>
+      </c>
+      <c r="G6">
+        <v>3821</v>
+      </c>
+      <c r="H6">
+        <v>3897</v>
+      </c>
+      <c r="I6">
+        <v>3935</v>
+      </c>
+      <c r="J6">
+        <v>3966</v>
+      </c>
+      <c r="K6">
+        <v>3985</v>
+      </c>
+      <c r="L6">
+        <v>4021</v>
+      </c>
+      <c r="M6">
+        <v>4078</v>
+      </c>
+      <c r="N6">
+        <v>4245</v>
+      </c>
+      <c r="O6">
+        <v>4792</v>
+      </c>
+      <c r="P6">
+        <v>4974</v>
+      </c>
+      <c r="Q6">
+        <v>5165</v>
+      </c>
+      <c r="R6">
+        <v>5289</v>
+      </c>
+      <c r="S6">
+        <v>5383</v>
+      </c>
+      <c r="T6">
+        <v>5458</v>
+      </c>
+      <c r="U6">
+        <v>5492</v>
+      </c>
+      <c r="V6">
+        <v>5594</v>
+      </c>
+      <c r="W6">
+        <v>5766</v>
+      </c>
+      <c r="X6">
+        <v>5953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2713</v>
+      </c>
+      <c r="C7">
+        <v>2850</v>
+      </c>
+      <c r="D7">
+        <v>3073</v>
+      </c>
+      <c r="E7">
+        <v>3292</v>
+      </c>
+      <c r="F7">
+        <v>3488</v>
+      </c>
+      <c r="G7">
+        <v>3734</v>
+      </c>
+      <c r="H7">
+        <v>3821</v>
+      </c>
+      <c r="I7">
+        <v>3897</v>
+      </c>
+      <c r="J7">
+        <v>3935</v>
+      </c>
+      <c r="K7">
+        <v>3966</v>
+      </c>
+      <c r="L7">
+        <v>3985</v>
+      </c>
+      <c r="M7">
+        <v>4021</v>
+      </c>
+      <c r="N7">
+        <v>4078</v>
+      </c>
+      <c r="O7">
+        <v>4519</v>
+      </c>
+      <c r="P7">
+        <v>4792</v>
+      </c>
+      <c r="Q7">
+        <v>4974</v>
+      </c>
+      <c r="R7">
+        <v>5165</v>
+      </c>
+      <c r="S7">
+        <v>5347</v>
+      </c>
+      <c r="T7">
+        <v>5417</v>
+      </c>
+      <c r="U7">
+        <v>5458</v>
+      </c>
+      <c r="V7">
+        <v>5492</v>
+      </c>
+      <c r="W7">
+        <v>5594</v>
+      </c>
+      <c r="X7">
+        <v>5766</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <v>223</v>
+      </c>
+      <c r="D8">
+        <v>219</v>
+      </c>
+      <c r="E8">
+        <v>196</v>
+      </c>
+      <c r="F8">
+        <v>246</v>
+      </c>
+      <c r="G8">
+        <v>87</v>
+      </c>
+      <c r="H8">
+        <v>76</v>
+      </c>
+      <c r="I8">
+        <v>38</v>
+      </c>
+      <c r="J8">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>19</v>
+      </c>
+      <c r="L8">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>57</v>
+      </c>
+      <c r="N8">
+        <v>167</v>
+      </c>
+      <c r="O8">
+        <v>273</v>
+      </c>
+      <c r="P8">
+        <v>182</v>
+      </c>
+      <c r="Q8">
+        <v>191</v>
+      </c>
+      <c r="R8">
+        <v>124</v>
+      </c>
+      <c r="S8">
+        <v>36</v>
+      </c>
+      <c r="T8">
+        <v>41</v>
+      </c>
+      <c r="U8">
+        <v>34</v>
+      </c>
+      <c r="V8">
+        <v>102</v>
+      </c>
+      <c r="W8">
+        <v>172</v>
+      </c>
+      <c r="X8">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="C9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="E9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="F9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="G9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="H9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="I9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="K9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="L9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="M9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="N9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="O9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="P9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="R9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="S9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="T9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="U9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="V9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="W9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="X9">
+        <v>1.0168999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>139.31530000000001</v>
+      </c>
+      <c r="C10">
+        <v>226.7687</v>
+      </c>
+      <c r="D10">
+        <v>222.7011</v>
+      </c>
+      <c r="E10">
+        <v>199.3124</v>
+      </c>
+      <c r="F10">
+        <v>250.1574</v>
+      </c>
+      <c r="G10">
+        <v>88.470299999999995</v>
+      </c>
+      <c r="H10">
+        <v>77.284400000000005</v>
+      </c>
+      <c r="I10">
+        <v>38.642200000000003</v>
+      </c>
+      <c r="J10">
+        <v>31.523900000000001</v>
+      </c>
+      <c r="K10">
+        <v>19.321100000000001</v>
+      </c>
+      <c r="L10">
+        <v>36.608400000000003</v>
+      </c>
+      <c r="M10">
+        <v>57.963299999999997</v>
+      </c>
+      <c r="N10">
+        <v>169.82230000000001</v>
+      </c>
+      <c r="O10">
+        <v>277.61369999999999</v>
+      </c>
+      <c r="P10">
+        <v>185.07579999999999</v>
+      </c>
+      <c r="Q10">
+        <v>194.22790000000001</v>
+      </c>
+      <c r="R10">
+        <v>126.0956</v>
+      </c>
+      <c r="S10">
+        <v>36.608400000000003</v>
+      </c>
+      <c r="T10">
+        <v>41.692900000000002</v>
+      </c>
+      <c r="U10">
+        <v>34.574599999999997</v>
+      </c>
+      <c r="V10">
+        <v>103.7238</v>
+      </c>
+      <c r="W10">
+        <v>174.9068</v>
+      </c>
+      <c r="X10">
+        <v>190.16030000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1.0215000000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.0388999999999999</v>
+      </c>
+      <c r="E11">
+        <v>1.0582</v>
+      </c>
+      <c r="F11">
+        <v>1.0375000000000001</v>
+      </c>
+      <c r="G11">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="H11">
+        <v>1.0254000000000001</v>
+      </c>
+      <c r="I11">
+        <v>1.022</v>
+      </c>
+      <c r="J11">
+        <v>1.0225</v>
+      </c>
+      <c r="K11">
+        <v>1.0215000000000001</v>
+      </c>
+      <c r="L11">
+        <v>1.0248999999999999</v>
+      </c>
+      <c r="M11">
+        <v>1.0337000000000001</v>
+      </c>
+      <c r="N11">
+        <v>1.0387</v>
+      </c>
+      <c r="O11">
+        <v>1.0362</v>
+      </c>
+      <c r="P11">
+        <v>1.0364</v>
+      </c>
+      <c r="Q11">
+        <v>1.0346</v>
+      </c>
+      <c r="R11">
+        <v>1.0265</v>
+      </c>
+      <c r="S11">
+        <v>1.0313000000000001</v>
+      </c>
+      <c r="T11">
+        <v>1.0238</v>
+      </c>
+      <c r="U11">
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="V11">
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="W11">
+        <v>1.0403</v>
+      </c>
+      <c r="X11">
+        <v>1.0403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>142.31057999999999</v>
+      </c>
+      <c r="C12">
+        <v>234.25207</v>
+      </c>
+      <c r="D12">
+        <v>231.36417</v>
+      </c>
+      <c r="E12">
+        <v>210.91238000000001</v>
+      </c>
+      <c r="F12">
+        <v>259.53829999999999</v>
+      </c>
+      <c r="G12">
+        <v>90.858999999999995</v>
+      </c>
+      <c r="H12">
+        <v>79.247420000000005</v>
+      </c>
+      <c r="I12">
+        <v>39.492330000000003</v>
+      </c>
+      <c r="J12">
+        <v>32.23319</v>
+      </c>
+      <c r="K12">
+        <v>19.736499999999999</v>
+      </c>
+      <c r="L12">
+        <v>37.519950000000001</v>
+      </c>
+      <c r="M12">
+        <v>59.91666</v>
+      </c>
+      <c r="N12">
+        <v>176.39442</v>
+      </c>
+      <c r="O12">
+        <v>287.66332</v>
+      </c>
+      <c r="P12">
+        <v>191.81255999999999</v>
+      </c>
+      <c r="Q12">
+        <v>200.94818000000001</v>
+      </c>
+      <c r="R12">
+        <v>129.43713</v>
+      </c>
+      <c r="S12">
+        <v>37.754240000000003</v>
+      </c>
+      <c r="T12">
+        <v>42.685189999999999</v>
+      </c>
+      <c r="U12">
+        <v>35.660240000000002</v>
+      </c>
+      <c r="V12">
+        <v>106.98072999999999</v>
+      </c>
+      <c r="W12">
+        <v>181.95554000000001</v>
+      </c>
+      <c r="X12">
+        <v>197.82375999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>218.95</v>
+      </c>
+      <c r="C13">
+        <v>360.4</v>
+      </c>
+      <c r="D13">
+        <v>355.95</v>
+      </c>
+      <c r="E13">
+        <v>324.49</v>
+      </c>
+      <c r="F13">
+        <v>399.3</v>
+      </c>
+      <c r="G13">
+        <v>139.72</v>
+      </c>
+      <c r="H13">
+        <v>122.24</v>
+      </c>
+      <c r="I13">
+        <v>61.36</v>
+      </c>
+      <c r="J13">
+        <v>49.89</v>
+      </c>
+      <c r="K13">
+        <v>30.59</v>
+      </c>
+      <c r="L13">
+        <v>58.02</v>
+      </c>
+      <c r="M13">
+        <v>93.16</v>
+      </c>
+      <c r="N13">
+        <v>275.25</v>
+      </c>
+      <c r="O13">
+        <v>454.32</v>
+      </c>
+      <c r="P13">
+        <v>313.76</v>
+      </c>
+      <c r="Q13">
+        <v>392.33</v>
+      </c>
+      <c r="R13">
+        <v>254.27</v>
+      </c>
+      <c r="S13">
+        <v>74.98</v>
+      </c>
+      <c r="T13">
+        <v>84.42</v>
+      </c>
+      <c r="U13">
+        <v>69.27</v>
+      </c>
+      <c r="V13">
+        <v>193.36</v>
+      </c>
+      <c r="W13">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="X13">
+        <v>355.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" t="s">
+        <v>15</v>
+      </c>
+      <c r="T14" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" t="s">
+        <v>15</v>
+      </c>
+      <c r="V14" t="s">
+        <v>15</v>
+      </c>
+      <c r="W14" t="s">
+        <v>15</v>
+      </c>
+      <c r="X14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>17</v>
+      </c>
+      <c r="R15" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" t="s">
+        <v>17</v>
+      </c>
+      <c r="T15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" t="s">
+        <v>17</v>
+      </c>
+      <c r="V15" t="s">
+        <v>17</v>
+      </c>
+      <c r="W15" t="s">
+        <v>17</v>
+      </c>
+      <c r="X15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.874</v>
+      </c>
+      <c r="C16">
+        <v>0.874</v>
+      </c>
+      <c r="D16">
+        <v>0.874</v>
+      </c>
+      <c r="E16">
+        <v>0.874</v>
+      </c>
+      <c r="F16">
+        <v>0.874</v>
+      </c>
+      <c r="G16">
+        <v>0.874</v>
+      </c>
+      <c r="H16">
+        <v>0.874</v>
+      </c>
+      <c r="I16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="L16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="M16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="N16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="O16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="P16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="R16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="S16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="T16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="U16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="V16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="W16">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="X16">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="C17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="D17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="F17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="H17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="I17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="J17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="K17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="L17">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="M17">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="N17">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="O17">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="P17">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="Q17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="S17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="T17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="U17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="V17">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="W17">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="X17">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="T18">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="U18">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="V18">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1.5385</v>
+      </c>
+      <c r="C19">
+        <v>1.5385</v>
+      </c>
+      <c r="D19">
+        <v>1.5385</v>
+      </c>
+      <c r="E19">
+        <v>1.5385</v>
+      </c>
+      <c r="F19">
+        <v>1.5385</v>
+      </c>
+      <c r="G19">
+        <v>1.5385</v>
+      </c>
+      <c r="H19">
+        <v>1.5385</v>
+      </c>
+      <c r="I19">
+        <v>1.5485</v>
+      </c>
+      <c r="J19">
+        <v>1.5485</v>
+      </c>
+      <c r="K19">
+        <v>1.5485</v>
+      </c>
+      <c r="L19">
+        <v>1.5485</v>
+      </c>
+      <c r="M19">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="N19">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="O19">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="P19">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="Q19">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="R19">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="S19">
+        <v>1.9755</v>
+      </c>
+      <c r="T19">
+        <v>1.9755</v>
+      </c>
+      <c r="U19">
+        <v>1.9755</v>
+      </c>
+      <c r="V19">
+        <v>1.8095000000000001</v>
+      </c>
+      <c r="W19">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="X19">
+        <v>1.7949999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="L20">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="P20">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="R20">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="U20">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="V20">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="L21">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="P21">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R21">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="U21">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="V21">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="U22">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23">
+        <v>1.5485</v>
+      </c>
+      <c r="L23">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="P23">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="R23">
+        <v>1.9635</v>
+      </c>
+      <c r="U23">
+        <v>1.8095000000000001</v>
+      </c>
+      <c r="V23">
+        <v>1.7949999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>218.95</v>
+      </c>
+      <c r="C24">
+        <v>360.4</v>
+      </c>
+      <c r="D24">
+        <v>355.95</v>
+      </c>
+      <c r="E24">
+        <v>324.49</v>
+      </c>
+      <c r="F24">
+        <v>399.3</v>
+      </c>
+      <c r="G24">
+        <v>139.72</v>
+      </c>
+      <c r="H24">
+        <v>122.24</v>
+      </c>
+      <c r="I24">
+        <v>61.36</v>
+      </c>
+      <c r="J24">
+        <v>49.89</v>
+      </c>
+      <c r="K24">
+        <v>30.59</v>
+      </c>
+      <c r="L24">
+        <v>58.02</v>
+      </c>
+      <c r="M24">
+        <v>93.16</v>
+      </c>
+      <c r="N24">
+        <v>275.25</v>
+      </c>
+      <c r="O24">
+        <v>454.32</v>
+      </c>
+      <c r="P24">
+        <v>313.76</v>
+      </c>
+      <c r="Q24">
+        <v>392.33</v>
+      </c>
+      <c r="R24">
+        <v>254.27</v>
+      </c>
+      <c r="S24">
+        <v>74.98</v>
+      </c>
+      <c r="T24">
+        <v>84.42</v>
+      </c>
+      <c r="U24">
+        <v>69.27</v>
+      </c>
+      <c r="V24">
+        <v>193.36</v>
+      </c>
+      <c r="W24">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="X24">
+        <v>355.09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>20.57</v>
+      </c>
+      <c r="C25">
+        <v>20.57</v>
+      </c>
+      <c r="D25">
+        <v>20.57</v>
+      </c>
+      <c r="E25">
+        <v>20.57</v>
+      </c>
+      <c r="F25">
+        <v>20.57</v>
+      </c>
+      <c r="G25">
+        <v>20.57</v>
+      </c>
+      <c r="H25">
+        <v>20.81</v>
+      </c>
+      <c r="I25">
+        <v>20.81</v>
+      </c>
+      <c r="J25">
+        <v>20.81</v>
+      </c>
+      <c r="K25">
+        <v>20.81</v>
+      </c>
+      <c r="L25">
+        <v>20.81</v>
+      </c>
+      <c r="M25">
+        <v>20.81</v>
+      </c>
+      <c r="N25">
+        <v>20.81</v>
+      </c>
+      <c r="O25">
+        <v>20.81</v>
+      </c>
+      <c r="P25">
+        <v>20.81</v>
+      </c>
+      <c r="Q25">
+        <v>20.81</v>
+      </c>
+      <c r="R25">
+        <v>20.81</v>
+      </c>
+      <c r="S25">
+        <v>21.1</v>
+      </c>
+      <c r="T25">
+        <v>21.1</v>
+      </c>
+      <c r="U25">
+        <v>21.1</v>
+      </c>
+      <c r="V25">
+        <v>21.1</v>
+      </c>
+      <c r="W25">
+        <v>21.1</v>
+      </c>
+      <c r="X25">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>239.52</v>
+      </c>
+      <c r="C26">
+        <v>380.97</v>
+      </c>
+      <c r="D26">
+        <v>376.52</v>
+      </c>
+      <c r="E26">
+        <v>345.06</v>
+      </c>
+      <c r="F26">
+        <v>419.87</v>
+      </c>
+      <c r="G26">
+        <v>160.29</v>
+      </c>
+      <c r="H26">
+        <v>143.05000000000001</v>
+      </c>
+      <c r="I26">
+        <v>82.17</v>
+      </c>
+      <c r="J26">
+        <v>70.7</v>
+      </c>
+      <c r="K26">
+        <v>51.4</v>
+      </c>
+      <c r="L26">
+        <v>78.83</v>
+      </c>
+      <c r="M26">
+        <v>113.97</v>
+      </c>
+      <c r="N26">
+        <v>296.06</v>
+      </c>
+      <c r="O26">
+        <v>475.13</v>
+      </c>
+      <c r="P26">
+        <v>334.57</v>
+      </c>
+      <c r="Q26">
+        <v>413.14</v>
+      </c>
+      <c r="R26">
+        <v>275.08</v>
+      </c>
+      <c r="S26">
+        <v>96.08</v>
+      </c>
+      <c r="T26">
+        <v>105.52</v>
+      </c>
+      <c r="U26">
+        <v>90.37</v>
+      </c>
+      <c r="V26">
+        <v>214.46</v>
+      </c>
+      <c r="W26">
+        <v>346.2</v>
+      </c>
+      <c r="X26">
+        <v>376.19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42738</v>
+      </c>
+      <c r="C28" s="1">
+        <v>42767</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42799</v>
+      </c>
+      <c r="E28" s="1">
+        <v>42827</v>
+      </c>
+      <c r="F28" s="1">
+        <v>42858</v>
+      </c>
+      <c r="G28" s="1">
+        <v>42886</v>
+      </c>
+      <c r="H28" s="1">
+        <v>42919</v>
+      </c>
+      <c r="I28" s="1">
+        <v>42953</v>
+      </c>
+      <c r="J28" s="1">
+        <v>42981</v>
+      </c>
+      <c r="K28" s="1">
+        <v>43012</v>
+      </c>
+      <c r="L28" s="1">
+        <v>43040</v>
+      </c>
+      <c r="M28" s="1">
+        <v>43072</v>
+      </c>
+      <c r="N28" s="1">
+        <v>43102</v>
+      </c>
+      <c r="O28" s="1">
+        <v>43164</v>
+      </c>
+      <c r="P28" s="1">
+        <v>43192</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>43222</v>
+      </c>
+      <c r="R28" s="1">
+        <v>43256</v>
+      </c>
+      <c r="S28" s="1">
+        <v>43317</v>
+      </c>
+      <c r="T28" s="1">
+        <v>43380</v>
+      </c>
+      <c r="U28" s="1">
+        <v>43404</v>
+      </c>
+      <c r="V28" s="1">
+        <v>43438</v>
+      </c>
+      <c r="W28" s="1">
+        <v>43467</v>
+      </c>
+      <c r="X28" s="1">
+        <v>43499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>128.52000000000001</v>
+      </c>
+      <c r="C29">
+        <v>239.52</v>
+      </c>
+      <c r="D29">
+        <v>620.49</v>
+      </c>
+      <c r="E29">
+        <v>134.52000000000001</v>
+      </c>
+      <c r="F29">
+        <v>345.06</v>
+      </c>
+      <c r="G29">
+        <v>419.87</v>
+      </c>
+      <c r="H29">
+        <v>160.29</v>
+      </c>
+      <c r="I29">
+        <v>143.05000000000001</v>
+      </c>
+      <c r="J29">
+        <v>82.17</v>
+      </c>
+      <c r="K29">
+        <v>70.7</v>
+      </c>
+      <c r="L29">
+        <v>51.4</v>
+      </c>
+      <c r="M29">
+        <v>78.83</v>
+      </c>
+      <c r="N29">
+        <v>112.8</v>
+      </c>
+      <c r="O29">
+        <v>474.61</v>
+      </c>
+      <c r="P29">
+        <v>475.13</v>
+      </c>
+      <c r="Q29">
+        <v>334.57</v>
+      </c>
+      <c r="R29">
+        <v>413.14</v>
+      </c>
+      <c r="S29">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="T29">
+        <v>91.54</v>
+      </c>
+      <c r="U29">
+        <v>105.52</v>
+      </c>
+      <c r="V29">
+        <v>195.89</v>
+      </c>
+      <c r="W29">
+        <v>108.83</v>
+      </c>
+      <c r="X29">
+        <v>346.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" t="s">
+        <v>42</v>
+      </c>
+      <c r="N30" t="s">
+        <v>41</v>
+      </c>
+      <c r="O30" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>38</v>
+      </c>
+      <c r="R30" t="s">
+        <v>37</v>
+      </c>
+      <c r="S30" t="s">
+        <v>36</v>
+      </c>
+      <c r="T30" t="s">
+        <v>35</v>
+      </c>
+      <c r="U30" t="s">
+        <v>34</v>
+      </c>
+      <c r="V30" t="s">
+        <v>33</v>
+      </c>
+      <c r="W30" t="s">
+        <v>54</v>
+      </c>
+      <c r="X30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1AADD3-2FA6-4EA9-B1C1-F0FC7B7DCD3A}">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection sqref="A1:X30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="24" width="15.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1">
         <v>43411</v>
@@ -5143,7 +7185,7 @@
         <v>43440</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5217,7 +7259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -5291,7 +7333,7 @@
         <v>43439</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -5365,7 +7407,7 @@
         <v>43409</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -5439,7 +7481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -5513,7 +7555,7 @@
         <v>5766</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -5587,7 +7629,7 @@
         <v>5594</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -5661,7 +7703,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -5735,7 +7777,7 @@
         <v>1.0168999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -5809,7 +7851,7 @@
         <v>174.9068</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5883,7 +7925,7 @@
         <v>1.0403</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -5957,7 +7999,7 @@
         <v>181.95554000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -6031,7 +8073,7 @@
         <v>325.10000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -6105,7 +8147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -6179,7 +8221,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -6253,7 +8295,7 @@
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -6327,7 +8369,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -6401,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -6475,7 +8517,7 @@
         <v>1.7949999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -6498,7 +8540,7 @@
         <v>0.88400000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -6521,7 +8563,7 @@
         <v>0.66449999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -6544,7 +8586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -6567,7 +8609,7 @@
         <v>1.5485</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -6641,7 +8683,7 @@
         <v>325.10000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -6715,7 +8757,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -6789,7 +8831,7 @@
         <v>346.2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -6863,7 +8905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -6937,7 +8979,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -7011,7 +9053,7 @@
         <v>108.83</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -7091,7 +9133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2607DA2E-F5D3-46D1-958D-9F994F975C89}">
   <dimension ref="A1:AH24"/>
   <sheetViews>
@@ -7099,45 +9141,45 @@
       <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.53515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.3828125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.3046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.3046875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.3828125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.3828125" customWidth="1"/>
     <col min="15" max="15" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.15234375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.3046875" customWidth="1"/>
+    <col min="24" max="24" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.3828125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.53515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7241,7 +9283,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>42711</v>
       </c>
@@ -7337,7 +9379,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>42740</v>
       </c>
@@ -7433,7 +9475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>42772</v>
       </c>
@@ -7529,7 +9571,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>42800</v>
       </c>
@@ -7625,7 +9667,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>42831</v>
       </c>
@@ -7721,7 +9763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>42859</v>
       </c>
@@ -7817,7 +9859,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>42892</v>
       </c>
@@ -7925,7 +9967,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>42926</v>
       </c>
@@ -8021,7 +10063,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>42954</v>
       </c>
@@ -8117,7 +10159,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>42985</v>
       </c>
@@ -8213,7 +10255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>43013</v>
       </c>
@@ -8321,7 +10363,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>43045</v>
       </c>
@@ -8417,7 +10459,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>43075</v>
       </c>
@@ -8513,7 +10555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>43137</v>
       </c>
@@ -8609,7 +10651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>43165</v>
       </c>
@@ -8717,7 +10759,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>43195</v>
       </c>
@@ -8813,7 +10855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>43229</v>
       </c>
@@ -8921,7 +10963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>43290</v>
       </c>
@@ -9017,7 +11059,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>43353</v>
       </c>
@@ -9113,7 +11155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>43377</v>
       </c>
@@ -9221,7 +11263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>43411</v>
       </c>
@@ -9329,7 +11371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>43440</v>
       </c>
@@ -9425,7 +11467,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>43472</v>
       </c>
@@ -9522,7 +11564,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:AH24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH24">
     <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9530,24 +11572,2078 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B8CE919-5A61-42F7-851B-97E1F4FD8DCC}">
+  <dimension ref="A1:AD24"/>
+  <sheetViews>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection sqref="A1:AD24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.61328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.23046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.23046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.61328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.61328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.15234375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.23046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.15234375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.921875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.4609375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.61328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A2" s="1">
+        <v>42711</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42709</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42677</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>2850</v>
+      </c>
+      <c r="G2">
+        <v>2713</v>
+      </c>
+      <c r="H2">
+        <v>137</v>
+      </c>
+      <c r="I2">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J2">
+        <v>139.31530000000001</v>
+      </c>
+      <c r="K2">
+        <v>1.0215000000000001</v>
+      </c>
+      <c r="L2">
+        <v>142.31057999999999</v>
+      </c>
+      <c r="M2">
+        <v>218.95</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2">
+        <v>0.874</v>
+      </c>
+      <c r="Q2">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1.5385</v>
+      </c>
+      <c r="X2">
+        <v>218.95</v>
+      </c>
+      <c r="Y2">
+        <v>20.57</v>
+      </c>
+      <c r="Z2">
+        <v>239.52</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>42738</v>
+      </c>
+      <c r="AC2">
+        <v>128.52000000000001</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A3" s="1">
+        <v>42740</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42739</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42709</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>3073</v>
+      </c>
+      <c r="G3">
+        <v>2850</v>
+      </c>
+      <c r="H3">
+        <v>223</v>
+      </c>
+      <c r="I3">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J3">
+        <v>226.7687</v>
+      </c>
+      <c r="K3">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="L3">
+        <v>234.25207</v>
+      </c>
+      <c r="M3">
+        <v>360.4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3">
+        <v>0.874</v>
+      </c>
+      <c r="Q3">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1.5385</v>
+      </c>
+      <c r="X3">
+        <v>360.4</v>
+      </c>
+      <c r="Y3">
+        <v>20.57</v>
+      </c>
+      <c r="Z3">
+        <v>380.97</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>42767</v>
+      </c>
+      <c r="AC3">
+        <v>239.52</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>42772</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42769</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42739</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>3292</v>
+      </c>
+      <c r="G4">
+        <v>3073</v>
+      </c>
+      <c r="H4">
+        <v>219</v>
+      </c>
+      <c r="I4">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J4">
+        <v>222.7011</v>
+      </c>
+      <c r="K4">
+        <v>1.0388999999999999</v>
+      </c>
+      <c r="L4">
+        <v>231.36417</v>
+      </c>
+      <c r="M4">
+        <v>355.95</v>
+      </c>
+      <c r="N4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4">
+        <v>0.874</v>
+      </c>
+      <c r="Q4">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1.5385</v>
+      </c>
+      <c r="X4">
+        <v>355.95</v>
+      </c>
+      <c r="Y4">
+        <v>20.57</v>
+      </c>
+      <c r="Z4">
+        <v>376.52</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>42799</v>
+      </c>
+      <c r="AC4">
+        <v>620.49</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>42800</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42797</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42769</v>
+      </c>
+      <c r="E5">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>3488</v>
+      </c>
+      <c r="G5">
+        <v>3292</v>
+      </c>
+      <c r="H5">
+        <v>196</v>
+      </c>
+      <c r="I5">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J5">
+        <v>199.3124</v>
+      </c>
+      <c r="K5">
+        <v>1.0582</v>
+      </c>
+      <c r="L5">
+        <v>210.91238000000001</v>
+      </c>
+      <c r="M5">
+        <v>324.49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5">
+        <v>0.874</v>
+      </c>
+      <c r="Q5">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1.5385</v>
+      </c>
+      <c r="X5">
+        <v>324.49</v>
+      </c>
+      <c r="Y5">
+        <v>20.57</v>
+      </c>
+      <c r="Z5">
+        <v>345.06</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>42827</v>
+      </c>
+      <c r="AC5">
+        <v>134.52000000000001</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>42831</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42830</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42797</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6">
+        <v>3734</v>
+      </c>
+      <c r="G6">
+        <v>3488</v>
+      </c>
+      <c r="H6">
+        <v>246</v>
+      </c>
+      <c r="I6">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J6">
+        <v>250.1574</v>
+      </c>
+      <c r="K6">
+        <v>1.0375000000000001</v>
+      </c>
+      <c r="L6">
+        <v>259.53829999999999</v>
+      </c>
+      <c r="M6">
+        <v>399.3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6">
+        <v>0.874</v>
+      </c>
+      <c r="Q6">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1.5385</v>
+      </c>
+      <c r="X6">
+        <v>399.3</v>
+      </c>
+      <c r="Y6">
+        <v>20.57</v>
+      </c>
+      <c r="Z6">
+        <v>419.87</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>42858</v>
+      </c>
+      <c r="AC6">
+        <v>345.06</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A7" s="1">
+        <v>42859</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42858</v>
+      </c>
+      <c r="D7" s="1">
+        <v>42830</v>
+      </c>
+      <c r="E7">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>3821</v>
+      </c>
+      <c r="G7">
+        <v>3734</v>
+      </c>
+      <c r="H7">
+        <v>87</v>
+      </c>
+      <c r="I7">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J7">
+        <v>88.470299999999995</v>
+      </c>
+      <c r="K7">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="L7">
+        <v>90.858999999999995</v>
+      </c>
+      <c r="M7">
+        <v>139.72</v>
+      </c>
+      <c r="N7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7">
+        <v>0.874</v>
+      </c>
+      <c r="Q7">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1.5385</v>
+      </c>
+      <c r="X7">
+        <v>139.72</v>
+      </c>
+      <c r="Y7">
+        <v>20.57</v>
+      </c>
+      <c r="Z7">
+        <v>160.29</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>42886</v>
+      </c>
+      <c r="AC7">
+        <v>419.87</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A8" s="1">
+        <v>42892</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42891</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42858</v>
+      </c>
+      <c r="E8">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>3897</v>
+      </c>
+      <c r="G8">
+        <v>3821</v>
+      </c>
+      <c r="H8">
+        <v>76</v>
+      </c>
+      <c r="I8">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J8">
+        <v>77.284400000000005</v>
+      </c>
+      <c r="K8">
+        <v>1.0254000000000001</v>
+      </c>
+      <c r="L8">
+        <v>79.247420000000005</v>
+      </c>
+      <c r="M8">
+        <v>122.24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8">
+        <v>0.874</v>
+      </c>
+      <c r="Q8">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1.5385</v>
+      </c>
+      <c r="T8">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="U8">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1.5485</v>
+      </c>
+      <c r="X8">
+        <v>122.24</v>
+      </c>
+      <c r="Y8">
+        <v>20.81</v>
+      </c>
+      <c r="Z8">
+        <v>143.05000000000001</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>42919</v>
+      </c>
+      <c r="AC8">
+        <v>160.29</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A9" s="1">
+        <v>42926</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42922</v>
+      </c>
+      <c r="D9" s="1">
+        <v>42891</v>
+      </c>
+      <c r="E9">
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <v>3935</v>
+      </c>
+      <c r="G9">
+        <v>3897</v>
+      </c>
+      <c r="H9">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J9">
+        <v>38.642200000000003</v>
+      </c>
+      <c r="K9">
+        <v>1.022</v>
+      </c>
+      <c r="L9">
+        <v>39.492330000000003</v>
+      </c>
+      <c r="M9">
+        <v>61.36</v>
+      </c>
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q9">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1.5485</v>
+      </c>
+      <c r="X9">
+        <v>61.36</v>
+      </c>
+      <c r="Y9">
+        <v>20.81</v>
+      </c>
+      <c r="Z9">
+        <v>82.17</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>42953</v>
+      </c>
+      <c r="AC9">
+        <v>143.05000000000001</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>42954</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42950</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42922</v>
+      </c>
+      <c r="E10">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>3966</v>
+      </c>
+      <c r="G10">
+        <v>3935</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+      <c r="I10">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J10">
+        <v>31.523900000000001</v>
+      </c>
+      <c r="K10">
+        <v>1.0225</v>
+      </c>
+      <c r="L10">
+        <v>32.23319</v>
+      </c>
+      <c r="M10">
+        <v>49.89</v>
+      </c>
+      <c r="N10" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q10">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1.5485</v>
+      </c>
+      <c r="X10">
+        <v>49.89</v>
+      </c>
+      <c r="Y10">
+        <v>20.81</v>
+      </c>
+      <c r="Z10">
+        <v>70.7</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>42981</v>
+      </c>
+      <c r="AC10">
+        <v>82.17</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A11" s="1">
+        <v>42985</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42984</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42950</v>
+      </c>
+      <c r="E11">
+        <v>34</v>
+      </c>
+      <c r="F11">
+        <v>3985</v>
+      </c>
+      <c r="G11">
+        <v>3966</v>
+      </c>
+      <c r="H11">
+        <v>19</v>
+      </c>
+      <c r="I11">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J11">
+        <v>19.321100000000001</v>
+      </c>
+      <c r="K11">
+        <v>1.0215000000000001</v>
+      </c>
+      <c r="L11">
+        <v>19.736499999999999</v>
+      </c>
+      <c r="M11">
+        <v>30.59</v>
+      </c>
+      <c r="N11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1.5485</v>
+      </c>
+      <c r="X11">
+        <v>30.59</v>
+      </c>
+      <c r="Y11">
+        <v>20.81</v>
+      </c>
+      <c r="Z11">
+        <v>51.4</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>43012</v>
+      </c>
+      <c r="AC11">
+        <v>70.7</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A12" s="1">
+        <v>43013</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43012</v>
+      </c>
+      <c r="D12" s="1">
+        <v>42984</v>
+      </c>
+      <c r="E12">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>4021</v>
+      </c>
+      <c r="G12">
+        <v>3985</v>
+      </c>
+      <c r="H12">
+        <v>36</v>
+      </c>
+      <c r="I12">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J12">
+        <v>36.608400000000003</v>
+      </c>
+      <c r="K12">
+        <v>1.0248999999999999</v>
+      </c>
+      <c r="L12">
+        <v>37.519950000000001</v>
+      </c>
+      <c r="M12">
+        <v>58.02</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q12">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1.5485</v>
+      </c>
+      <c r="T12">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="U12">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="X12">
+        <v>58.02</v>
+      </c>
+      <c r="Y12">
+        <v>20.81</v>
+      </c>
+      <c r="Z12">
+        <v>78.83</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>43040</v>
+      </c>
+      <c r="AC12">
+        <v>51.4</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A13" s="1">
+        <v>43045</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43042</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43012</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>4078</v>
+      </c>
+      <c r="G13">
+        <v>4021</v>
+      </c>
+      <c r="H13">
+        <v>57</v>
+      </c>
+      <c r="I13">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J13">
+        <v>57.963299999999997</v>
+      </c>
+      <c r="K13">
+        <v>1.0337000000000001</v>
+      </c>
+      <c r="L13">
+        <v>59.91666</v>
+      </c>
+      <c r="M13">
+        <v>93.16</v>
+      </c>
+      <c r="N13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q13">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="X13">
+        <v>93.16</v>
+      </c>
+      <c r="Y13">
+        <v>20.81</v>
+      </c>
+      <c r="Z13">
+        <v>113.97</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>43072</v>
+      </c>
+      <c r="AC13">
+        <v>78.83</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A14" s="1">
+        <v>43075</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43074</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43042</v>
+      </c>
+      <c r="E14">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>4245</v>
+      </c>
+      <c r="G14">
+        <v>4078</v>
+      </c>
+      <c r="H14">
+        <v>167</v>
+      </c>
+      <c r="I14">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J14">
+        <v>169.82230000000001</v>
+      </c>
+      <c r="K14">
+        <v>1.0387</v>
+      </c>
+      <c r="L14">
+        <v>176.39442</v>
+      </c>
+      <c r="M14">
+        <v>275.25</v>
+      </c>
+      <c r="N14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" t="s">
+        <v>17</v>
+      </c>
+      <c r="P14">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q14">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="X14">
+        <v>275.25</v>
+      </c>
+      <c r="Y14">
+        <v>20.81</v>
+      </c>
+      <c r="Z14">
+        <v>296.06</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>43102</v>
+      </c>
+      <c r="AC14">
+        <v>112.8</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A15" s="1">
+        <v>43137</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43136</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43103</v>
+      </c>
+      <c r="E15">
+        <v>33</v>
+      </c>
+      <c r="F15">
+        <v>4792</v>
+      </c>
+      <c r="G15">
+        <v>4519</v>
+      </c>
+      <c r="H15">
+        <v>273</v>
+      </c>
+      <c r="I15">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J15">
+        <v>277.61369999999999</v>
+      </c>
+      <c r="K15">
+        <v>1.0362</v>
+      </c>
+      <c r="L15">
+        <v>287.66332</v>
+      </c>
+      <c r="M15">
+        <v>454.32</v>
+      </c>
+      <c r="N15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q15">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="X15">
+        <v>454.32</v>
+      </c>
+      <c r="Y15">
+        <v>20.81</v>
+      </c>
+      <c r="Z15">
+        <v>475.13</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>43164</v>
+      </c>
+      <c r="AC15">
+        <v>474.61</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A16" s="1">
+        <v>43165</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43164</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43136</v>
+      </c>
+      <c r="E16">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <v>4974</v>
+      </c>
+      <c r="G16">
+        <v>4792</v>
+      </c>
+      <c r="H16">
+        <v>182</v>
+      </c>
+      <c r="I16">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J16">
+        <v>185.07579999999999</v>
+      </c>
+      <c r="K16">
+        <v>1.0364</v>
+      </c>
+      <c r="L16">
+        <v>191.81255999999999</v>
+      </c>
+      <c r="M16">
+        <v>313.76</v>
+      </c>
+      <c r="N16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>17</v>
+      </c>
+      <c r="P16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q16">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1.5680000000000001</v>
+      </c>
+      <c r="T16">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="U16">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="X16">
+        <v>313.76</v>
+      </c>
+      <c r="Y16">
+        <v>20.81</v>
+      </c>
+      <c r="Z16">
+        <v>334.57</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>43192</v>
+      </c>
+      <c r="AC16">
+        <v>475.13</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A17" s="1">
+        <v>43195</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43194</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43164</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>5165</v>
+      </c>
+      <c r="G17">
+        <v>4974</v>
+      </c>
+      <c r="H17">
+        <v>191</v>
+      </c>
+      <c r="I17">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J17">
+        <v>194.22790000000001</v>
+      </c>
+      <c r="K17">
+        <v>1.0346</v>
+      </c>
+      <c r="L17">
+        <v>200.94818000000001</v>
+      </c>
+      <c r="M17">
+        <v>392.33</v>
+      </c>
+      <c r="N17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="X17">
+        <v>392.33</v>
+      </c>
+      <c r="Y17">
+        <v>20.81</v>
+      </c>
+      <c r="Z17">
+        <v>413.14</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>43222</v>
+      </c>
+      <c r="AC17">
+        <v>334.57</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A18" s="1">
+        <v>43229</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43223</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43194</v>
+      </c>
+      <c r="E18">
+        <v>29</v>
+      </c>
+      <c r="F18">
+        <v>5289</v>
+      </c>
+      <c r="G18">
+        <v>5165</v>
+      </c>
+      <c r="H18">
+        <v>124</v>
+      </c>
+      <c r="I18">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J18">
+        <v>126.0956</v>
+      </c>
+      <c r="K18">
+        <v>1.0265</v>
+      </c>
+      <c r="L18">
+        <v>129.43713</v>
+      </c>
+      <c r="M18">
+        <v>254.27</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P18">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="Q18">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="T18">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="U18">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="V18">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="W18">
+        <v>1.9635</v>
+      </c>
+      <c r="X18">
+        <v>254.27</v>
+      </c>
+      <c r="Y18">
+        <v>20.81</v>
+      </c>
+      <c r="Z18">
+        <v>275.08</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>43256</v>
+      </c>
+      <c r="AC18">
+        <v>413.14</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A19" s="1">
+        <v>43290</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43286</v>
+      </c>
+      <c r="D19" s="1">
+        <v>43256</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>5383</v>
+      </c>
+      <c r="G19">
+        <v>5347</v>
+      </c>
+      <c r="H19">
+        <v>36</v>
+      </c>
+      <c r="I19">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J19">
+        <v>36.608400000000003</v>
+      </c>
+      <c r="K19">
+        <v>1.0313000000000001</v>
+      </c>
+      <c r="L19">
+        <v>37.754240000000003</v>
+      </c>
+      <c r="M19">
+        <v>74.98</v>
+      </c>
+      <c r="N19" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q19">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R19">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="S19">
+        <v>1.9755</v>
+      </c>
+      <c r="X19">
+        <v>74.98</v>
+      </c>
+      <c r="Y19">
+        <v>21.1</v>
+      </c>
+      <c r="Z19">
+        <v>96.08</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>43317</v>
+      </c>
+      <c r="AC19">
+        <v>140.08000000000001</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A20" s="1">
+        <v>43353</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43349</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43315</v>
+      </c>
+      <c r="E20">
+        <v>34</v>
+      </c>
+      <c r="F20">
+        <v>5458</v>
+      </c>
+      <c r="G20">
+        <v>5417</v>
+      </c>
+      <c r="H20">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J20">
+        <v>41.692900000000002</v>
+      </c>
+      <c r="K20">
+        <v>1.0238</v>
+      </c>
+      <c r="L20">
+        <v>42.685189999999999</v>
+      </c>
+      <c r="M20">
+        <v>84.42</v>
+      </c>
+      <c r="N20" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q20">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R20">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="S20">
+        <v>1.9755</v>
+      </c>
+      <c r="X20">
+        <v>84.42</v>
+      </c>
+      <c r="Y20">
+        <v>21.1</v>
+      </c>
+      <c r="Z20">
+        <v>105.52</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>43380</v>
+      </c>
+      <c r="AC20">
+        <v>91.54</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A21" s="1">
+        <v>43377</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43376</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43349</v>
+      </c>
+      <c r="E21">
+        <v>27</v>
+      </c>
+      <c r="F21">
+        <v>5492</v>
+      </c>
+      <c r="G21">
+        <v>5458</v>
+      </c>
+      <c r="H21">
+        <v>34</v>
+      </c>
+      <c r="I21">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J21">
+        <v>34.574599999999997</v>
+      </c>
+      <c r="K21">
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="L21">
+        <v>35.660240000000002</v>
+      </c>
+      <c r="M21">
+        <v>69.27</v>
+      </c>
+      <c r="N21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q21">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="R21">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="S21">
+        <v>1.9755</v>
+      </c>
+      <c r="T21">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="U21">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="V21">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="W21">
+        <v>1.8095000000000001</v>
+      </c>
+      <c r="X21">
+        <v>69.27</v>
+      </c>
+      <c r="Y21">
+        <v>21.1</v>
+      </c>
+      <c r="Z21">
+        <v>90.37</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>43404</v>
+      </c>
+      <c r="AC21">
+        <v>105.52</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A22" s="1">
+        <v>43411</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43409</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43376</v>
+      </c>
+      <c r="E22">
+        <v>33</v>
+      </c>
+      <c r="F22">
+        <v>5594</v>
+      </c>
+      <c r="G22">
+        <v>5492</v>
+      </c>
+      <c r="H22">
+        <v>102</v>
+      </c>
+      <c r="I22">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J22">
+        <v>103.7238</v>
+      </c>
+      <c r="K22">
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="L22">
+        <v>106.98072999999999</v>
+      </c>
+      <c r="M22">
+        <v>193.36</v>
+      </c>
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q22">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R22">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="S22">
+        <v>1.8095000000000001</v>
+      </c>
+      <c r="T22">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="U22">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="X22">
+        <v>193.36</v>
+      </c>
+      <c r="Y22">
+        <v>21.1</v>
+      </c>
+      <c r="Z22">
+        <v>214.46</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>43438</v>
+      </c>
+      <c r="AC22">
+        <v>195.89</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>43440</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43439</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43409</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>5766</v>
+      </c>
+      <c r="G23">
+        <v>5594</v>
+      </c>
+      <c r="H23">
+        <v>172</v>
+      </c>
+      <c r="I23">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J23">
+        <v>174.9068</v>
+      </c>
+      <c r="K23">
+        <v>1.0403</v>
+      </c>
+      <c r="L23">
+        <v>181.95554000000001</v>
+      </c>
+      <c r="M23">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="N23" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q23">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="X23">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="Y23">
+        <v>21.1</v>
+      </c>
+      <c r="Z23">
+        <v>346.2</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>43467</v>
+      </c>
+      <c r="AC23">
+        <v>108.83</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>43472</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43469</v>
+      </c>
+      <c r="D24" s="1">
+        <v>43439</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>5953</v>
+      </c>
+      <c r="G24">
+        <v>5766</v>
+      </c>
+      <c r="H24">
+        <v>187</v>
+      </c>
+      <c r="I24">
+        <v>1.0168999999999999</v>
+      </c>
+      <c r="J24">
+        <v>190.16030000000001</v>
+      </c>
+      <c r="K24">
+        <v>1.0403</v>
+      </c>
+      <c r="L24">
+        <v>197.82375999999999</v>
+      </c>
+      <c r="M24">
+        <v>355.09</v>
+      </c>
+      <c r="N24" t="s">
+        <v>15</v>
+      </c>
+      <c r="O24" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="Q24">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="X24">
+        <v>355.09</v>
+      </c>
+      <c r="Y24">
+        <v>21.1</v>
+      </c>
+      <c r="Z24">
+        <v>376.19</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>43499</v>
+      </c>
+      <c r="AC24">
+        <v>346.2</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD24">
+    <sortCondition ref="A2:A24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD0A928-B657-412F-8DAC-4E02179F4730}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.15234375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -9564,7 +13660,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -9578,7 +13674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -9595,7 +13691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -9612,7 +13708,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>71</v>
       </c>

</xml_diff>